<commit_message>
Kiegeszitettuk a 8 kodblokkot gyujtesi alkalom szerinti es honaponkenti befogott fajok szerinti felbontassal
</commit_message>
<xml_diff>
--- a/tipulidae_eredmenyek.xlsx
+++ b/tipulidae_eredmenyek.xlsx
@@ -20,12 +20,15 @@
     <sheet name="Campia Romana" r:id="rId14" sheetId="12"/>
     <sheet name="Subcarpatii" r:id="rId15" sheetId="13"/>
     <sheet name="Regionkenti adatok" r:id="rId16" sheetId="14"/>
+    <sheet name="Honaponkent gyujtott egyedek" r:id="rId17" sheetId="15"/>
+    <sheet name="Honaponkenti gyujtesi alkalmak" r:id="rId18" sheetId="16"/>
+    <sheet name="Honaponkenti befogott fajok" r:id="rId19" sheetId="17"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8300" uniqueCount="1390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8384" uniqueCount="1402">
   <si>
     <t>id</t>
   </si>
@@ -4195,6 +4198,42 @@
   </si>
   <si>
     <t>Subcarpatii</t>
+  </si>
+  <si>
+    <t>jan</t>
+  </si>
+  <si>
+    <t>feb</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>apr</t>
+  </si>
+  <si>
+    <t>maj</t>
+  </si>
+  <si>
+    <t>jun</t>
+  </si>
+  <si>
+    <t>jul</t>
+  </si>
+  <si>
+    <t>aug</t>
+  </si>
+  <si>
+    <t>sep</t>
+  </si>
+  <si>
+    <t>okt</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>dec</t>
   </si>
 </sst>
 </file>
@@ -8324,6 +8363,2130 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>328.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>138.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>489.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>136.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>160.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>234.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
A honaponkenti fajok szama regionkent lekerdezest javitottuk a 8 kodblokkba
</commit_message>
<xml_diff>
--- a/tipulidae_eredmenyek.xlsx
+++ b/tipulidae_eredmenyek.xlsx
@@ -10194,13 +10194,13 @@
         <v>0.0</v>
       </c>
       <c r="F3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="I3" t="n">
         <v>0.0</v>
@@ -10232,25 +10232,25 @@
         <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="F4" t="n">
-        <v>107.0</v>
+        <v>37.0</v>
       </c>
       <c r="G4" t="n">
-        <v>56.0</v>
+        <v>24.0</v>
       </c>
       <c r="H4" t="n">
-        <v>234.0</v>
+        <v>48.0</v>
       </c>
       <c r="I4" t="n">
-        <v>44.0</v>
+        <v>17.0</v>
       </c>
       <c r="J4" t="n">
-        <v>24.0</v>
+        <v>9.0</v>
       </c>
       <c r="K4" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="L4" t="n">
         <v>2.0</v>
@@ -10273,25 +10273,25 @@
         <v>1.0</v>
       </c>
       <c r="E5" t="n">
-        <v>27.0</v>
+        <v>10.0</v>
       </c>
       <c r="F5" t="n">
-        <v>66.0</v>
+        <v>26.0</v>
       </c>
       <c r="G5" t="n">
-        <v>47.0</v>
+        <v>30.0</v>
       </c>
       <c r="H5" t="n">
-        <v>25.0</v>
+        <v>13.0</v>
       </c>
       <c r="I5" t="n">
-        <v>23.0</v>
+        <v>13.0</v>
       </c>
       <c r="J5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K5" t="n">
         <v>5.0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>7.0</v>
       </c>
       <c r="L5" t="n">
         <v>2.0</v>
@@ -10317,7 +10317,7 @@
         <v>3.0</v>
       </c>
       <c r="F6" t="n">
-        <v>15.0</v>
+        <v>12.0</v>
       </c>
       <c r="G6" t="n">
         <v>2.0</v>
@@ -10326,7 +10326,7 @@
         <v>4.0</v>
       </c>
       <c r="I6" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="J6" t="n">
         <v>1.0</v>
@@ -10355,25 +10355,25 @@
         <v>0.0</v>
       </c>
       <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I7" t="n">
         <v>4.0</v>
       </c>
-      <c r="F7" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>5.0</v>
-      </c>
       <c r="J7" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="K7" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="L7" t="n">
         <v>1.0</v>
@@ -10440,7 +10440,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" t="n">
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
       <c r="G9" t="n">
         <v>2.0</v>
@@ -10481,16 +10481,16 @@
         <v>0.0</v>
       </c>
       <c r="F10" t="n">
-        <v>46.0</v>
+        <v>32.0</v>
       </c>
       <c r="G10" t="n">
-        <v>49.0</v>
+        <v>33.0</v>
       </c>
       <c r="H10" t="n">
-        <v>18.0</v>
+        <v>16.0</v>
       </c>
       <c r="I10" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="J10" t="n">
         <v>0.0</v>
@@ -10522,16 +10522,16 @@
         <v>0.0</v>
       </c>
       <c r="F11" t="n">
-        <v>15.0</v>
+        <v>11.0</v>
       </c>
       <c r="G11" t="n">
         <v>3.0</v>
       </c>
       <c r="H11" t="n">
-        <v>13.0</v>
+        <v>9.0</v>
       </c>
       <c r="I11" t="n">
-        <v>13.0</v>
+        <v>8.0</v>
       </c>
       <c r="J11" t="n">
         <v>1.0</v>
@@ -10645,10 +10645,10 @@
         <v>1.0</v>
       </c>
       <c r="F14" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="G14" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="H14" t="n">
         <v>0.0</v>
@@ -10657,7 +10657,7 @@
         <v>0.0</v>
       </c>
       <c r="J14" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="K14" t="n">
         <v>0.0</v>
@@ -10689,7 +10689,7 @@
         <v>0.0</v>
       </c>
       <c r="G15" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="H15" t="n">
         <v>0.0</v>

</xml_diff>